<commit_message>
More Openpyxl Learning - to develop actual real file
These are variuos files I have created to help me develop my program for working with Excel. Been painfully good!!
</commit_message>
<xml_diff>
--- a/Openpyxl Tutorial/chart.xlsx
+++ b/Openpyxl Tutorial/chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16787\Documents\GitHub\Excel-Python-Playing-Together\Excel-Python-Playing-Together\Openpyxl Tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE8F6FF-1EB3-4947-AC9F-733D2DBFC780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C695C3D-CCFC-4862-BB90-B8469C213FD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5684,7 +5684,7 @@
   <dimension ref="A1:W70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>